<commit_message>
Zadanie 103, 104, wskazniki w notatkach
</commit_message>
<xml_diff>
--- a/maturainformatyka.xlsx
+++ b/maturainformatyka.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Desktop\Informatyka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Desktop\Informatyka\MaturaZadania\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Zadania</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>wszystkie</t>
+  </si>
+  <si>
+    <t>Problem z importem</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{01A7F9A6-67CD-442E-8B0B-7B409BD56429}" diskRevisions="1" revisionId="11" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7EA9DBBA-EEC4-4417-B10F-50AA89112EF2}" diskRevisions="1" revisionId="13" version="6">
   <header guid="{7F0CB6CC-6FF8-414D-A8D4-F20750B94300}" dateTime="2017-02-08T21:04:39" maxSheetId="2" userName="Piotrek K" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -218,6 +221,16 @@
     </sheetIdMap>
   </header>
   <header guid="{01A7F9A6-67CD-442E-8B0B-7B409BD56429}" dateTime="2017-02-10T20:07:05" maxSheetId="2" userName="Piotrek K" r:id="rId4" minRId="8" maxRId="11">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B3887188-DB7A-4E30-A350-5A072147D58C}" dateTime="2017-02-20T21:41:58" maxSheetId="2" userName="Piotrek K" r:id="rId5" minRId="12">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7EA9DBBA-EEC4-4417-B10F-50AA89112EF2}" dateTime="2017-02-20T22:02:57" maxSheetId="2" userName="Piotrek K" r:id="rId6" minRId="13">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -298,6 +311,28 @@
     </oc>
     <nc r="H16">
       <f>112-58</f>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="12" sId="1" numFmtId="19">
+    <nc r="D47">
+      <v>42786</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="13" sId="1">
+    <nc r="E48" t="inlineStr">
+      <is>
+        <t>Problem z importem</t>
+      </is>
     </nc>
   </rcc>
 </revisions>
@@ -596,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,14 +665,14 @@
       </c>
       <c r="F1" s="6">
         <f>(H16-H15)/H16</f>
-        <v>0.27777777777777779</v>
+        <v>0.29629629629629628</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="7">
         <f ca="1">H15/H11</f>
-        <v>0.43820224719101125</v>
+        <v>0.48101265822784811</v>
       </c>
       <c r="I1" t="s">
         <v>13</v>
@@ -774,7 +809,7 @@
       </c>
       <c r="H11" s="5">
         <f ca="1">DATEDIF(TODAY(), H10, "d")</f>
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -792,7 +827,7 @@
       </c>
       <c r="H12">
         <f ca="1">TRUNC(RAND()*55)+58</f>
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -836,7 +871,7 @@
       </c>
       <c r="H15">
         <f>COUNTBLANK(D2:D56)</f>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -1185,7 +1220,9 @@
       <c r="C47" s="3">
         <v>42769</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3">
+        <v>42786</v>
+      </c>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -1196,7 +1233,9 @@
         <v>42770</v>
       </c>
       <c r="D48" s="3"/>
-      <c r="E48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="2">

</xml_diff>

<commit_message>
Zadanie 65, modyfikacja 64
</commit_message>
<xml_diff>
--- a/maturainformatyka.xlsx
+++ b/maturainformatyka.xlsx
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7EA9DBBA-EEC4-4417-B10F-50AA89112EF2}" diskRevisions="1" revisionId="13" version="6">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{15A2D96C-F774-4500-8F3B-80EE6390CEB7}" diskRevisions="1" revisionId="14" version="7">
   <header guid="{7F0CB6CC-6FF8-414D-A8D4-F20750B94300}" dateTime="2017-02-08T21:04:39" maxSheetId="2" userName="Piotrek K" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -231,6 +231,11 @@
     </sheetIdMap>
   </header>
   <header guid="{7EA9DBBA-EEC4-4417-B10F-50AA89112EF2}" dateTime="2017-02-20T22:02:57" maxSheetId="2" userName="Piotrek K" r:id="rId6" minRId="13">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{15A2D96C-F774-4500-8F3B-80EE6390CEB7}" dateTime="2017-02-21T18:50:36" maxSheetId="2" userName="Piotrek K" r:id="rId7" minRId="14">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -333,6 +338,16 @@
       <is>
         <t>Problem z importem</t>
       </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="14" sId="1" numFmtId="19">
+    <nc r="D9">
+      <v>42787</v>
     </nc>
   </rcc>
 </revisions>
@@ -631,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,14 +680,14 @@
       </c>
       <c r="F1" s="6">
         <f>(H16-H15)/H16</f>
-        <v>0.29629629629629628</v>
+        <v>0.31481481481481483</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="7">
         <f ca="1">H15/H11</f>
-        <v>0.48101265822784811</v>
+        <v>0.47435897435897434</v>
       </c>
       <c r="I1" t="s">
         <v>13</v>
@@ -775,7 +790,9 @@
       <c r="C9" s="3">
         <v>42731</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3">
+        <v>42787</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -809,7 +826,7 @@
       </c>
       <c r="H11" s="5">
         <f ca="1">DATEDIF(TODAY(), H10, "d")</f>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -827,7 +844,7 @@
       </c>
       <c r="H12">
         <f ca="1">TRUNC(RAND()*55)+58</f>
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -871,7 +888,7 @@
       </c>
       <c r="H15">
         <f>COUNTBLANK(D2:D56)</f>
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>